<commit_message>
Fix column order for Birthdays sheet in Excel export
</commit_message>
<xml_diff>
--- a/pycalendar_data.xlsx
+++ b/pycalendar_data.xlsx
@@ -724,17 +724,17 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Grid Color</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Text Color</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Description</t>
         </is>
       </c>
     </row>
@@ -746,17 +746,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>Ahmet's Birthday</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>#87CEFA</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>#000000</t>
-        </is>
-      </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Ahmet's Birthday</t>
+          <t>#000000</t>
         </is>
       </c>
     </row>
@@ -768,17 +768,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>Buse's Birthday</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>#87CEFA</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>#000000</t>
-        </is>
-      </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Buse's Birthday</t>
+          <t>#000000</t>
         </is>
       </c>
     </row>
@@ -790,17 +790,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>Mehmet's Birthday</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
           <t>#87CEFA</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>#000000</t>
-        </is>
-      </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Mehmet's Birthday</t>
+          <t>#000000</t>
         </is>
       </c>
     </row>

</xml_diff>